<commit_message>
Looking at expanding arrays with IFNA,IFERROR
</commit_message>
<xml_diff>
--- a/CH-122 Table Transformation.xlsx
+++ b/CH-122 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23506F2-4475-49F6-867B-821C01EE5447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB33B201-01D0-42B2-9FA8-4D94657FD225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="33">
   <si>
     <t>Result</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>result</t>
+  </si>
+  <si>
+    <t>Mark</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Tim</t>
   </si>
 </sst>
 </file>
@@ -3060,10 +3069,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F9F6636-27EC-424E-86DE-FDDC5A982CB6}">
-  <dimension ref="C1:Y60"/>
+  <dimension ref="C1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M29" workbookViewId="0">
-      <selection activeCell="T41" sqref="T41"/>
+    <sheetView tabSelected="1" topLeftCell="M45" workbookViewId="0">
+      <selection activeCell="U63" sqref="U63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4638,25 +4647,71 @@
       <c r="O54">
         <v>1</v>
       </c>
+      <c r="V54" t="str" cm="1">
+        <f t="array" ref="V54:X58">_xlfn.IFNA(_xlfn.ANCHORARRAY(M31),{3,4,5})</f>
+        <v>19/09/2024</v>
+      </c>
+      <c r="W54" t="str">
+        <v>19/09/2024</v>
+      </c>
+      <c r="X54" t="str">
+        <v>19/09/2024</v>
+      </c>
     </row>
     <row r="55" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O55" t="str">
         <v>Apple</v>
       </c>
+      <c r="V55" t="str">
+        <v>19/09/2024</v>
+      </c>
+      <c r="W55" t="str">
+        <v>19/09/2024</v>
+      </c>
+      <c r="X55" t="str">
+        <v>19/09/2024</v>
+      </c>
     </row>
     <row r="56" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O56">
         <v>131</v>
+      </c>
+      <c r="V56" t="str">
+        <v>19/09/2024</v>
+      </c>
+      <c r="W56" t="str">
+        <v>19/09/2024</v>
+      </c>
+      <c r="X56" t="str">
+        <v>19/09/2024</v>
       </c>
     </row>
     <row r="57" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O57" t="str">
         <v>Mango</v>
       </c>
+      <c r="V57" t="str">
+        <v>17/09/2024</v>
+      </c>
+      <c r="W57" t="str">
+        <v>17/09/2024</v>
+      </c>
+      <c r="X57" t="str">
+        <v>17/09/2024</v>
+      </c>
     </row>
     <row r="58" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O58">
         <v>28</v>
+      </c>
+      <c r="V58" t="str">
+        <v>16/09/2024</v>
+      </c>
+      <c r="W58" t="str">
+        <v>16/09/2024</v>
+      </c>
+      <c r="X58" t="str">
+        <v>16/09/2024</v>
       </c>
     </row>
     <row r="59" spans="15:24" x14ac:dyDescent="0.25">
@@ -4667,6 +4722,77 @@
     <row r="60" spans="15:24" x14ac:dyDescent="0.25">
       <c r="O60">
         <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="15:24" x14ac:dyDescent="0.25">
+      <c r="Q64" t="s">
+        <v>30</v>
+      </c>
+      <c r="R64" t="str" cm="1">
+        <f t="array" ref="R64:T66">_xlfn.EXPAND(Q64:Q66,3,3)</f>
+        <v>Mark</v>
+      </c>
+      <c r="S64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T64" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V64" t="str" cm="1">
+        <f t="array" ref="V64:X66">IFERROR(Q64:Q66,{1,2,3})</f>
+        <v>Mark</v>
+      </c>
+      <c r="W64" t="str">
+        <v>Mark</v>
+      </c>
+      <c r="X64" t="str">
+        <v>Mark</v>
+      </c>
+    </row>
+    <row r="65" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q65" t="s">
+        <v>31</v>
+      </c>
+      <c r="R65" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="S65" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T65" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V65" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="W65" t="str">
+        <v>Craig</v>
+      </c>
+      <c r="X65" t="str">
+        <v>Craig</v>
+      </c>
+    </row>
+    <row r="66" spans="17:24" x14ac:dyDescent="0.25">
+      <c r="Q66" t="s">
+        <v>32</v>
+      </c>
+      <c r="R66" t="str">
+        <v>Tim</v>
+      </c>
+      <c r="S66" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T66" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="V66" t="str">
+        <v>Tim</v>
+      </c>
+      <c r="W66" t="str">
+        <v>Tim</v>
+      </c>
+      <c r="X66" t="str">
+        <v>Tim</v>
       </c>
     </row>
   </sheetData>

</xml_diff>